<commit_message>
predictive analysis pdf and recommendations
</commit_message>
<xml_diff>
--- a/EcoPulse-Data.xlsx
+++ b/EcoPulse-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUP\ECOPULSE\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F69314-7EE4-487F-83B1-F6781344E81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D48DC4D-5E60-4311-ABD0-10B4DABBA62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20986" windowHeight="13333" xr2:uid="{26AE0E1D-6678-480D-9AE9-572D51A0CD43}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Year</t>
   </si>
@@ -187,12 +187,6 @@
   </si>
   <si>
     <t>Bohol (Wind (GWh))</t>
-  </si>
-  <si>
-    <t>MERALCO Rate (PHP/kWh)</t>
-  </si>
-  <si>
-    <t>Solar Cost (PHP/W)</t>
   </si>
 </sst>
 </file>
@@ -578,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB78A2D4-B7C1-48A0-B50B-22BE5A359217}">
-  <dimension ref="A1:BA27"/>
+  <dimension ref="A1:AY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AZ10" sqref="AZ10"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BB22" sqref="BB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -635,7 +629,7 @@
     <col min="53" max="53" width="22.05859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,14 +783,8 @@
       <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2003</v>
       </c>
@@ -830,14 +818,8 @@
       <c r="K2" s="1">
         <v>7845677.42575741</v>
       </c>
-      <c r="AZ2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>5.2</v>
-      </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2004</v>
       </c>
@@ -872,14 +854,8 @@
         <v>8361077.9042326389</v>
       </c>
       <c r="M3" s="3"/>
-      <c r="AZ3">
-        <v>0</v>
-      </c>
-      <c r="BA3">
-        <v>5.3</v>
-      </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2005</v>
       </c>
@@ -1033,14 +1009,8 @@
       <c r="AY4">
         <v>0</v>
       </c>
-      <c r="AZ4">
-        <v>495</v>
-      </c>
-      <c r="BA4">
-        <v>5.5</v>
-      </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>2006</v>
       </c>
@@ -1194,14 +1164,8 @@
       <c r="AY5">
         <v>0</v>
       </c>
-      <c r="AZ5">
-        <v>433</v>
-      </c>
-      <c r="BA5">
-        <v>5.8</v>
-      </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2007</v>
       </c>
@@ -1355,14 +1319,8 @@
       <c r="AY6">
         <v>0</v>
       </c>
-      <c r="AZ6" s="1">
-        <v>368</v>
-      </c>
-      <c r="BA6" s="1">
-        <v>6</v>
-      </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>2008</v>
       </c>
@@ -1516,14 +1474,8 @@
       <c r="AY7">
         <v>0</v>
       </c>
-      <c r="AZ7" s="1">
-        <v>330</v>
-      </c>
-      <c r="BA7" s="1">
-        <v>6.5</v>
-      </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -1677,14 +1629,8 @@
       <c r="AY8">
         <v>0</v>
       </c>
-      <c r="AZ8" s="1">
-        <v>336</v>
-      </c>
-      <c r="BA8" s="1">
-        <v>6.8</v>
-      </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -1838,14 +1784,8 @@
       <c r="AY9">
         <v>0</v>
       </c>
-      <c r="AZ9" s="1">
-        <v>292</v>
-      </c>
-      <c r="BA9" s="1">
-        <v>7</v>
-      </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -1999,14 +1939,8 @@
       <c r="AY10">
         <v>0</v>
       </c>
-      <c r="AZ10" s="1">
-        <v>258</v>
-      </c>
-      <c r="BA10" s="1">
-        <v>7.5</v>
-      </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -2160,14 +2094,8 @@
       <c r="AY11">
         <v>0</v>
       </c>
-      <c r="AZ11" s="1">
-        <v>231</v>
-      </c>
-      <c r="BA11" s="1">
-        <v>8</v>
-      </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>2013</v>
       </c>
@@ -2321,14 +2249,8 @@
       <c r="AY12">
         <v>0</v>
       </c>
-      <c r="AZ12" s="1">
-        <v>210</v>
-      </c>
-      <c r="BA12" s="1">
-        <v>8.5</v>
-      </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2014</v>
       </c>
@@ -2482,14 +2404,8 @@
       <c r="AY13">
         <v>0</v>
       </c>
-      <c r="AZ13" s="1">
-        <v>198</v>
-      </c>
-      <c r="BA13" s="1">
-        <v>9</v>
-      </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -2643,14 +2559,8 @@
       <c r="AY14">
         <v>0</v>
       </c>
-      <c r="AZ14" s="1">
-        <v>188</v>
-      </c>
-      <c r="BA14" s="1">
-        <v>9.1999999999999993</v>
-      </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -2804,14 +2714,8 @@
       <c r="AY15">
         <v>0</v>
       </c>
-      <c r="AZ15" s="1">
-        <v>168</v>
-      </c>
-      <c r="BA15" s="1">
-        <v>9.5</v>
-      </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2017</v>
       </c>
@@ -2965,14 +2869,8 @@
       <c r="AY16">
         <v>0</v>
       </c>
-      <c r="AZ16" s="1">
-        <v>150</v>
-      </c>
-      <c r="BA16" s="1">
-        <v>9.8000000000000007</v>
-      </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2018</v>
       </c>
@@ -3126,14 +3024,8 @@
       <c r="AY17">
         <v>0</v>
       </c>
-      <c r="AZ17" s="1">
-        <v>132</v>
-      </c>
-      <c r="BA17" s="1">
-        <v>10</v>
-      </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -3287,14 +3179,8 @@
       <c r="AY18">
         <v>0</v>
       </c>
-      <c r="AZ18" s="1">
-        <v>109</v>
-      </c>
-      <c r="BA18" s="1">
-        <v>10.199999999999999</v>
-      </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -3448,14 +3334,8 @@
       <c r="AY19">
         <v>0</v>
       </c>
-      <c r="AZ19" s="1">
-        <v>85.5</v>
-      </c>
-      <c r="BA19" s="1">
-        <v>10.5</v>
-      </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -3609,14 +3489,8 @@
       <c r="AY20">
         <v>0</v>
       </c>
-      <c r="AZ20" s="1">
-        <v>69.5</v>
-      </c>
-      <c r="BA20" s="1">
-        <v>10.8</v>
-      </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>2022</v>
       </c>
@@ -3770,14 +3644,8 @@
       <c r="AY21">
         <v>0</v>
       </c>
-      <c r="AZ21" s="1">
-        <v>71.5</v>
-      </c>
-      <c r="BA21" s="1">
-        <v>11</v>
-      </c>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>2023</v>
       </c>
@@ -3931,20 +3799,14 @@
       <c r="AY22">
         <v>0</v>
       </c>
-      <c r="AZ22" s="1">
-        <v>61.5</v>
-      </c>
-      <c r="BA22" s="1">
-        <v>11.5</v>
-      </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.5">
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.5">
       <c r="L24" s="3"/>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.5">
       <c r="AJ27" t="s">
         <v>35</v>
       </c>

</xml_diff>